<commit_message>
Results from July 4, 2020 10:03 PM CT run
</commit_message>
<xml_diff>
--- a/workflow/python/output/xlsx/covid_disparities_output_2020-07-04.xlsx
+++ b/workflow/python/output/xlsx/covid_disparities_output_2020-07-04.xlsx
@@ -551,21 +551,39 @@
           <t>North Carolina</t>
         </is>
       </c>
-      <c r="B4" t="inlineStr"/>
-      <c r="C4" t="inlineStr"/>
-      <c r="D4" t="inlineStr"/>
-      <c r="E4" t="inlineStr"/>
-      <c r="F4" t="inlineStr"/>
-      <c r="G4" t="inlineStr"/>
-      <c r="H4" t="inlineStr"/>
+      <c r="B4" s="2" t="n">
+        <v>44016</v>
+      </c>
+      <c r="C4" t="n">
+        <v>71654</v>
+      </c>
+      <c r="D4" t="n">
+        <v>1395</v>
+      </c>
+      <c r="E4" t="n">
+        <v>11390</v>
+      </c>
+      <c r="F4" t="n">
+        <v>446</v>
+      </c>
+      <c r="G4" t="n">
+        <v>22.98</v>
+      </c>
+      <c r="H4" t="n">
+        <v>33.16</v>
+      </c>
       <c r="I4" t="b">
         <v>0</v>
       </c>
       <c r="J4" t="b">
-        <v>0</v>
-      </c>
-      <c r="K4" t="inlineStr"/>
-      <c r="L4" t="inlineStr"/>
+        <v>1</v>
+      </c>
+      <c r="K4" t="n">
+        <v>49566</v>
+      </c>
+      <c r="L4" t="n">
+        <v>1345</v>
+      </c>
       <c r="M4" t="n">
         <v>2179622</v>
       </c>
@@ -574,7 +592,7 @@
       </c>
       <c r="O4" t="inlineStr">
         <is>
-          <t>An error occurred. ... TimeoutException('', None, None)</t>
+          <t>Success!</t>
         </is>
       </c>
     </row>

</xml_diff>